<commit_message>
update weekly progress doc
</commit_message>
<xml_diff>
--- a/personal-logs/weekly-summary.xlsx
+++ b/personal-logs/weekly-summary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nwray\Documents\MDS\capstone\w2020-data599-capstone-projects-ubc-udl\personal-logs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8570787C-195E-4B8C-8A94-F71FCA09E78E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C96A31-AA25-4FB2-B9B8-6A74389F858E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
@@ -162,12 +162,418 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="31">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -175,7 +581,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -188,9 +594,66 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="6" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="30" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,7 +937,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -647,8 +1110,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69694E70-DF1C-4718-B283-3623588A95EF}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -691,7 +1154,7 @@
         <v>8</v>
       </c>
       <c r="F2" s="2">
-        <f>E2/$E$9</f>
+        <f t="shared" ref="F2:F9" si="0">E2/$E$9</f>
         <v>5.7866184448462928E-2</v>
       </c>
     </row>
@@ -709,11 +1172,11 @@
         <v>5.25</v>
       </c>
       <c r="E3" s="1">
-        <f t="shared" ref="E3:E8" si="0">SUM(B3:D3)</f>
+        <f t="shared" ref="E3:E8" si="1">SUM(B3:D3)</f>
         <v>16.75</v>
       </c>
       <c r="F3" s="2">
-        <f>E3/$E$9</f>
+        <f t="shared" si="0"/>
         <v>0.12115732368896925</v>
       </c>
     </row>
@@ -731,11 +1194,11 @@
         <v>7.5</v>
       </c>
       <c r="E4" s="1">
+        <f t="shared" si="1"/>
+        <v>42.5</v>
+      </c>
+      <c r="F4" s="2">
         <f t="shared" si="0"/>
-        <v>42.5</v>
-      </c>
-      <c r="F4" s="2">
-        <f>E4/$E$9</f>
         <v>0.30741410488245929</v>
       </c>
     </row>
@@ -751,11 +1214,11 @@
       </c>
       <c r="D5" s="5"/>
       <c r="E5" s="6">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
+      <c r="F5" s="7">
         <f t="shared" si="0"/>
-        <v>27</v>
-      </c>
-      <c r="F5" s="7">
-        <f>E5/$E$9</f>
         <v>0.19529837251356238</v>
       </c>
     </row>
@@ -767,11 +1230,11 @@
         <v>18</v>
       </c>
       <c r="E6" s="1">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="F6" s="2">
         <f t="shared" si="0"/>
-        <v>18</v>
-      </c>
-      <c r="F6" s="2">
-        <f>E6/$E$9</f>
         <v>0.1301989150090416</v>
       </c>
     </row>
@@ -783,11 +1246,11 @@
         <v>1</v>
       </c>
       <c r="E7" s="1">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="F7" s="2">
         <f t="shared" si="0"/>
-        <v>1</v>
-      </c>
-      <c r="F7" s="2">
-        <f>E7/$E$9</f>
         <v>7.2332730560578659E-3</v>
       </c>
     </row>
@@ -799,11 +1262,11 @@
         <v>25</v>
       </c>
       <c r="E8" s="1">
+        <f t="shared" si="1"/>
+        <v>25</v>
+      </c>
+      <c r="F8" s="2">
         <f t="shared" si="0"/>
-        <v>25</v>
-      </c>
-      <c r="F8" s="2">
-        <f>E8/$E$9</f>
         <v>0.18083182640144665</v>
       </c>
     </row>
@@ -828,7 +1291,7 @@
         <v>138.25</v>
       </c>
       <c r="F9" s="2">
-        <f>E9/$E$9</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
@@ -848,275 +1311,270 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74BA6663-D16A-4104-9460-16D01A5CF5FE}">
-  <dimension ref="A1:F17"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="49.21875" customWidth="1"/>
-    <col min="2" max="3" width="8.88671875" customWidth="1"/>
+    <col min="1" max="1" width="49.88671875" customWidth="1"/>
+    <col min="2" max="4" width="8.88671875" customWidth="1"/>
     <col min="5" max="5" width="14.109375" customWidth="1"/>
     <col min="6" max="6" width="12.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="28" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="32" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="33" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
+      <c r="A2" s="34" t="s">
         <v>5</v>
       </c>
-      <c r="B2">
+      <c r="B2" s="20">
         <v>8</v>
       </c>
-      <c r="C2">
+      <c r="C2" s="14">
         <v>7</v>
       </c>
-      <c r="D2">
+      <c r="D2" s="16">
         <v>2</v>
       </c>
-      <c r="E2" s="1">
+      <c r="E2" s="24">
         <f>SUM(B2:D2)</f>
         <v>17</v>
       </c>
-      <c r="F2" s="2">
-        <f>E2/$E$15</f>
+      <c r="F2" s="15">
+        <f t="shared" ref="F2:F8" si="0">E2/$E$12</f>
         <v>0.11021069692058347</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+      <c r="A3" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="21">
         <v>8</v>
       </c>
-      <c r="C3">
+      <c r="C3" s="8">
         <v>8.25</v>
       </c>
-      <c r="D3">
+      <c r="D3" s="17">
         <v>7.5</v>
       </c>
-      <c r="E3" s="1">
-        <f t="shared" ref="E3:E8" si="0">SUM(B3:D3)</f>
+      <c r="E3" s="25">
+        <f t="shared" ref="E3:E8" si="1">SUM(B3:D3)</f>
         <v>23.75</v>
       </c>
-      <c r="F3" s="2">
-        <f>E3/$E$15</f>
+      <c r="F3" s="9">
+        <f t="shared" si="0"/>
         <v>0.1539708265802269</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="3" t="s">
+      <c r="A4" s="36" t="s">
         <v>16</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="21">
         <v>16</v>
       </c>
-      <c r="E4" s="1">
+      <c r="C4" s="8"/>
+      <c r="D4" s="17"/>
+      <c r="E4" s="25">
+        <f t="shared" si="1"/>
+        <v>16</v>
+      </c>
+      <c r="F4" s="9">
         <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="F4" s="2">
-        <f>E4/$E$15</f>
         <v>0.10372771474878444</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
+      <c r="A5" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="5">
+      <c r="B5" s="22">
         <v>2.75</v>
       </c>
-      <c r="C5" s="5">
+      <c r="C5" s="10">
         <v>7</v>
       </c>
-      <c r="D5" s="5"/>
-      <c r="E5" s="6">
+      <c r="D5" s="18"/>
+      <c r="E5" s="26">
+        <f t="shared" si="1"/>
+        <v>9.75</v>
+      </c>
+      <c r="F5" s="11">
         <f t="shared" si="0"/>
-        <v>9.75</v>
-      </c>
-      <c r="F5" s="7">
-        <f>E5/$E$15</f>
         <v>6.3209076175040513E-2</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+      <c r="A6" s="35" t="s">
         <v>20</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="21">
         <v>4</v>
       </c>
-      <c r="E6" s="1">
+      <c r="C6" s="8"/>
+      <c r="D6" s="17"/>
+      <c r="E6" s="25">
+        <f t="shared" si="1"/>
+        <v>4</v>
+      </c>
+      <c r="F6" s="9">
         <f t="shared" si="0"/>
+        <v>2.5931928687196109E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="35" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="21">
+        <v>0.75</v>
+      </c>
+      <c r="C7" s="8">
+        <v>3</v>
+      </c>
+      <c r="D7" s="17"/>
+      <c r="E7" s="25">
+        <f t="shared" si="1"/>
+        <v>3.75</v>
+      </c>
+      <c r="F7" s="9">
+        <f t="shared" si="0"/>
+        <v>2.4311183144246355E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A8" s="38" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="23">
         <v>4</v>
       </c>
-      <c r="F6" s="2">
-        <f>E6/$E$15</f>
-        <v>2.5931928687196109E-2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7">
-        <v>0.75</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="E7" s="1">
+      <c r="C8" s="12">
+        <v>11.5</v>
+      </c>
+      <c r="D8" s="19">
+        <v>31.25</v>
+      </c>
+      <c r="E8" s="27">
+        <f t="shared" si="1"/>
+        <v>46.75</v>
+      </c>
+      <c r="F8" s="13">
         <f t="shared" si="0"/>
-        <v>3.75</v>
-      </c>
-      <c r="F7" s="2">
-        <f>E7/$E$15</f>
-        <v>2.4311183144246355E-2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="8" t="s">
+        <v>0.30307941653160453</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A9" s="35" t="s">
+        <v>18</v>
+      </c>
+      <c r="B9" s="21">
+        <v>2</v>
+      </c>
+      <c r="C9" s="8"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="25">
+        <f t="shared" ref="E9:E11" si="2">SUM(B9:D9)</f>
+        <v>2</v>
+      </c>
+      <c r="F9" s="9">
+        <f t="shared" ref="F9:F11" si="3">E9/$E$12</f>
+        <v>1.2965964343598054E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="39" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="22">
         <v>19</v>
       </c>
-      <c r="B8" s="8">
+      <c r="C10" s="10">
         <v>4</v>
       </c>
-      <c r="C8" s="8">
-        <v>11.5</v>
-      </c>
-      <c r="D8" s="8">
-        <v>31.25</v>
-      </c>
-      <c r="E8" s="9">
-        <f t="shared" si="0"/>
-        <v>46.75</v>
-      </c>
-      <c r="F8" s="10">
-        <f>E8/$E$15</f>
-        <v>0.30307941653160453</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9">
-        <v>2</v>
-      </c>
-      <c r="E9" s="1">
-        <f t="shared" ref="E9:E11" si="1">SUM(B9:D9)</f>
-        <v>2</v>
-      </c>
-      <c r="F9" s="2">
-        <f t="shared" ref="F9:F11" si="2">E9/$E$15</f>
-        <v>1.2965964343598054E-2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="5">
-        <v>19</v>
-      </c>
-      <c r="C10" s="5">
+      <c r="D10" s="18"/>
+      <c r="E10" s="26">
+        <f t="shared" si="2"/>
+        <v>23</v>
+      </c>
+      <c r="F10" s="11">
+        <f t="shared" si="3"/>
+        <v>0.14910858995137763</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="B11" s="47">
+        <v>0.25</v>
+      </c>
+      <c r="C11" s="48">
+        <v>8</v>
+      </c>
+      <c r="D11" s="49"/>
+      <c r="E11" s="50">
+        <f t="shared" si="2"/>
+        <v>8.25</v>
+      </c>
+      <c r="F11" s="51">
+        <f t="shared" si="3"/>
+        <v>5.3484602917341979E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="D10" s="5"/>
-      <c r="E10" s="6">
-        <f t="shared" si="1"/>
-        <v>23</v>
-      </c>
-      <c r="F10" s="7">
-        <f t="shared" si="2"/>
-        <v>0.14910858995137763</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B11" s="5">
-        <v>0.25</v>
-      </c>
-      <c r="C11" s="5">
-        <v>8</v>
-      </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="6">
-        <f t="shared" si="1"/>
-        <v>8.25</v>
-      </c>
-      <c r="F11" s="7">
-        <f t="shared" si="2"/>
-        <v>5.3484602917341979E-2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E12" s="1"/>
-      <c r="F12" s="2"/>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E13" s="1"/>
-      <c r="F13" s="2"/>
+      <c r="B12" s="41">
+        <f>SUM(B2:B11)</f>
+        <v>64.75</v>
+      </c>
+      <c r="C12" s="42">
+        <f>SUM(C2:C11)</f>
+        <v>48.75</v>
+      </c>
+      <c r="D12" s="43">
+        <f>SUM(D2:D11)</f>
+        <v>40.75</v>
+      </c>
+      <c r="E12" s="44">
+        <f>SUM(E2:E11)</f>
+        <v>154.25</v>
+      </c>
+      <c r="F12" s="45">
+        <f>E12/$E$12</f>
+        <v>1</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="E14" s="1"/>
-      <c r="F14" s="2"/>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B15" s="1">
-        <f>SUM(B2:B14)</f>
-        <v>64.75</v>
-      </c>
-      <c r="C15" s="1">
-        <f>SUM(C2:C14)</f>
-        <v>48.75</v>
-      </c>
-      <c r="D15" s="1">
-        <f>SUM(D2:D14)</f>
-        <v>40.75</v>
-      </c>
-      <c r="E15" s="1">
-        <f>SUM(E2:E14)</f>
-        <v>154.25</v>
-      </c>
-      <c r="F15" s="2">
-        <f>E15/$E$15</f>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A17" s="1" t="s">
+      <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B14" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update summary and progress docs
</commit_message>
<xml_diff>
--- a/personal-logs/weekly-summary.xlsx
+++ b/personal-logs/weekly-summary.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nwray\Documents\MDS\capstone\w2020-data599-capstone-projects-ubc-udl\personal-logs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nwray\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0C96A31-AA25-4FB2-B9B8-6A74389F858E}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{136C8235-F445-4449-8EC9-E25C6D0BE3EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Week 1" sheetId="1" r:id="rId1"/>
     <sheet name="Week 2" sheetId="2" r:id="rId2"/>
     <sheet name="Week 3" sheetId="3" r:id="rId3"/>
+    <sheet name="Week 4" sheetId="4" r:id="rId4"/>
+    <sheet name="Week 5" sheetId="5" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm.Print_Area" localSheetId="3">'Week 4'!$A$1:$F$11</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="4">'Week 5'!$A$1:$F$8</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -27,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="30">
   <si>
     <t>Task</t>
   </si>
@@ -71,9 +77,6 @@
     <t>Parsing with Telegraf to support UDL</t>
   </si>
   <si>
-    <t>None</t>
-  </si>
-  <si>
     <t>Anomaly Detection Research / Testing Packages</t>
   </si>
   <si>
@@ -96,6 +99,30 @@
   </si>
   <si>
     <t>Manual Data Downloads</t>
+  </si>
+  <si>
+    <t>Items not considered in project proposal</t>
+  </si>
+  <si>
+    <t>Anomaly Labelling / Data Access</t>
+  </si>
+  <si>
+    <t>Status Presentation</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>Build Model Pipeline (Code/Research)</t>
+  </si>
+  <si>
+    <t>Evaluate Preliminary Results</t>
+  </si>
+  <si>
+    <t>Implement Model</t>
+  </si>
+  <si>
+    <t>Model Tuning/Results</t>
   </si>
 </sst>
 </file>
@@ -162,7 +189,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="31">
+  <borders count="37">
     <border>
       <left/>
       <right/>
@@ -572,6 +599,92 @@
       </right>
       <top/>
       <bottom style="medium">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="medium">
+        <color auto="1"/>
+      </right>
+      <top style="medium">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
         <color auto="1"/>
       </bottom>
       <diagonal/>
@@ -581,7 +694,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="9" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -654,6 +767,18 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="4" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="34" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="36" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -937,7 +1062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
@@ -1111,7 +1236,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A18" sqref="A18"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1182,7 +1307,7 @@
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4">
         <v>29.5</v>
@@ -1224,7 +1349,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C6">
         <v>18</v>
@@ -1256,7 +1381,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8">
         <v>25</v>
@@ -1299,8 +1424,8 @@
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" t="s">
-        <v>14</v>
+      <c r="B11" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1314,7 +1439,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1391,7 +1516,7 @@
     </row>
     <row r="4" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A4" s="36" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B4" s="21">
         <v>16</v>
@@ -1429,7 +1554,7 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="35" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B6" s="21">
         <v>4</v>
@@ -1467,7 +1592,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="38" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B8" s="23">
         <v>4</v>
@@ -1489,7 +1614,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="35" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B9" s="21">
         <v>2</v>
@@ -1507,7 +1632,7 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="39" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B10" s="22">
         <v>19</v>
@@ -1527,7 +1652,7 @@
     </row>
     <row r="11" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="46" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B11" s="47">
         <v>0.25</v>
@@ -1574,12 +1699,452 @@
       <c r="A14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B14" t="s">
-        <v>14</v>
+      <c r="B14" s="5" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5992D2D6-042E-410C-A59B-1F6FF45F9B6A}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:F11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="49.88671875" customWidth="1"/>
+    <col min="2" max="4" width="8.88671875" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" customWidth="1"/>
+    <col min="6" max="6" width="12.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="33" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="53">
+        <v>5</v>
+      </c>
+      <c r="C2" s="54">
+        <v>0.5</v>
+      </c>
+      <c r="D2" s="55">
+        <v>0</v>
+      </c>
+      <c r="E2" s="56">
+        <f>SUM(B2:D2)</f>
+        <v>5.5</v>
+      </c>
+      <c r="F2" s="57">
+        <f t="shared" ref="F2:F9" si="0">E2/$E$9</f>
+        <v>3.6727879799666109E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="21">
+        <v>5.5</v>
+      </c>
+      <c r="C3" s="8">
+        <v>5.5</v>
+      </c>
+      <c r="D3" s="17">
+        <v>6.25</v>
+      </c>
+      <c r="E3" s="25">
+        <f t="shared" ref="E3:E8" si="1">SUM(B3:D3)</f>
+        <v>17.25</v>
+      </c>
+      <c r="F3" s="9">
+        <f t="shared" si="0"/>
+        <v>0.11519198664440734</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="21">
+        <v>4.25</v>
+      </c>
+      <c r="C4" s="8">
+        <v>0</v>
+      </c>
+      <c r="D4" s="17">
+        <v>0</v>
+      </c>
+      <c r="E4" s="25">
+        <f t="shared" si="1"/>
+        <v>4.25</v>
+      </c>
+      <c r="F4" s="9">
+        <f t="shared" si="0"/>
+        <v>2.8380634390651086E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="23">
+        <v>2</v>
+      </c>
+      <c r="C5" s="12">
+        <v>0.5</v>
+      </c>
+      <c r="D5" s="19">
+        <v>0</v>
+      </c>
+      <c r="E5" s="27">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="F5" s="13">
+        <f t="shared" si="0"/>
+        <v>1.6694490818030049E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="35" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="21">
+        <v>24.5</v>
+      </c>
+      <c r="C6" s="8">
+        <v>31</v>
+      </c>
+      <c r="D6" s="17">
+        <v>34.25</v>
+      </c>
+      <c r="E6" s="25">
+        <f t="shared" si="1"/>
+        <v>89.75</v>
+      </c>
+      <c r="F6" s="9">
+        <f t="shared" si="0"/>
+        <v>0.59933222036727885</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A7" s="35" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="21">
+        <v>8.75</v>
+      </c>
+      <c r="C7" s="8">
+        <v>15</v>
+      </c>
+      <c r="D7" s="17">
+        <v>0</v>
+      </c>
+      <c r="E7" s="25">
+        <f t="shared" si="1"/>
+        <v>23.75</v>
+      </c>
+      <c r="F7" s="9">
+        <f t="shared" si="0"/>
+        <v>0.15859766277128548</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="46" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="47">
+        <v>6.75</v>
+      </c>
+      <c r="C8" s="48">
+        <v>0</v>
+      </c>
+      <c r="D8" s="49">
+        <v>0</v>
+      </c>
+      <c r="E8" s="50">
+        <f t="shared" si="1"/>
+        <v>6.75</v>
+      </c>
+      <c r="F8" s="51">
+        <f t="shared" si="0"/>
+        <v>4.5075125208681135E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" s="41">
+        <f>SUM(B2:B8)</f>
+        <v>56.75</v>
+      </c>
+      <c r="C9" s="42">
+        <f>SUM(C2:C8)</f>
+        <v>52.5</v>
+      </c>
+      <c r="D9" s="43">
+        <f>SUM(D2:D8)</f>
+        <v>40.5</v>
+      </c>
+      <c r="E9" s="44">
+        <f>SUM(E2:E8)</f>
+        <v>149.75</v>
+      </c>
+      <c r="F9" s="45">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{81A268A7-E39B-4ABC-99E2-BF28BEA00254}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:F10"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="49.88671875" customWidth="1"/>
+    <col min="2" max="4" width="8.88671875" customWidth="1"/>
+    <col min="5" max="5" width="14.109375" customWidth="1"/>
+    <col min="6" max="6" width="12.21875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="30" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="31" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="33" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="52" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="53">
+        <v>4.25</v>
+      </c>
+      <c r="C2" s="54">
+        <v>0.75</v>
+      </c>
+      <c r="D2" s="55">
+        <v>0</v>
+      </c>
+      <c r="E2" s="56">
+        <f>SUM(B2:D2)</f>
+        <v>5</v>
+      </c>
+      <c r="F2" s="57">
+        <f t="shared" ref="F2:F8" si="0">E2/$E$8</f>
+        <v>3.9525691699604744E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A3" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="21">
+        <v>6</v>
+      </c>
+      <c r="C3" s="8">
+        <v>5</v>
+      </c>
+      <c r="D3" s="17">
+        <v>3.25</v>
+      </c>
+      <c r="E3" s="25">
+        <f t="shared" ref="E3:E7" si="1">SUM(B3:D3)</f>
+        <v>14.25</v>
+      </c>
+      <c r="F3" s="9">
+        <f t="shared" si="0"/>
+        <v>0.11264822134387352</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="B4" s="21">
+        <v>6.25</v>
+      </c>
+      <c r="C4" s="8">
+        <v>8</v>
+      </c>
+      <c r="D4" s="17">
+        <v>3</v>
+      </c>
+      <c r="E4" s="25">
+        <f t="shared" si="1"/>
+        <v>17.25</v>
+      </c>
+      <c r="F4" s="9">
+        <f t="shared" si="0"/>
+        <v>0.13636363636363635</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A5" s="36" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="23">
+        <v>26</v>
+      </c>
+      <c r="C5" s="12">
+        <v>0</v>
+      </c>
+      <c r="D5" s="19">
+        <v>0</v>
+      </c>
+      <c r="E5" s="27">
+        <f t="shared" si="1"/>
+        <v>26</v>
+      </c>
+      <c r="F5" s="13">
+        <f t="shared" si="0"/>
+        <v>0.20553359683794467</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="35" t="s">
+        <v>28</v>
+      </c>
+      <c r="B6" s="21">
+        <v>0.5</v>
+      </c>
+      <c r="C6" s="8">
+        <v>0</v>
+      </c>
+      <c r="D6" s="17">
+        <v>34</v>
+      </c>
+      <c r="E6" s="25">
+        <f t="shared" si="1"/>
+        <v>34.5</v>
+      </c>
+      <c r="F6" s="9">
+        <f t="shared" si="0"/>
+        <v>0.27272727272727271</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="58" t="s">
+        <v>29</v>
+      </c>
+      <c r="B7" s="59">
+        <v>1.5</v>
+      </c>
+      <c r="C7" s="60">
+        <v>28</v>
+      </c>
+      <c r="D7" s="61">
+        <v>0</v>
+      </c>
+      <c r="E7" s="62">
+        <f t="shared" si="1"/>
+        <v>29.5</v>
+      </c>
+      <c r="F7" s="63">
+        <f t="shared" si="0"/>
+        <v>0.233201581027668</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="41">
+        <f>SUM(B2:B7)</f>
+        <v>44.5</v>
+      </c>
+      <c r="C8" s="42">
+        <f>SUM(C2:C7)</f>
+        <v>41.75</v>
+      </c>
+      <c r="D8" s="43">
+        <f>SUM(D2:D7)</f>
+        <v>40.25</v>
+      </c>
+      <c r="E8" s="44">
+        <f>SUM(E2:E7)</f>
+        <v>126.5</v>
+      </c>
+      <c r="F8" s="45">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10" s="5"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="landscape" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>